<commit_message>
R2.01 changed C5, C6, C7
</commit_message>
<xml_diff>
--- a/BOM/electronicloadBOM.xlsx
+++ b/BOM/electronicloadBOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="36" windowWidth="22980" windowHeight="9552"/>
+    <workbookView xWindow="0" yWindow="36" windowWidth="22980" windowHeight="9552" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="electronicloadBOM" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="84">
   <si>
     <t>Qty</t>
   </si>
@@ -59,12 +59,6 @@
     <t>100n</t>
   </si>
   <si>
-    <t>C0603K</t>
-  </si>
-  <si>
-    <t>C2, C4, C5, C6</t>
-  </si>
-  <si>
     <t>CAPACITOR, European symbol</t>
   </si>
   <si>
@@ -77,9 +71,6 @@
     <t>1u</t>
   </si>
   <si>
-    <t>C1, C3</t>
-  </si>
-  <si>
     <t>20k</t>
   </si>
   <si>
@@ -264,6 +255,18 @@
   </si>
   <si>
     <t>N-Channel HEXFET Power MOSFET Logic Level</t>
+  </si>
+  <si>
+    <t>C1, C3, C5, C6</t>
+  </si>
+  <si>
+    <t>C0603</t>
+  </si>
+  <si>
+    <t>C2, C4, C7</t>
+  </si>
+  <si>
+    <t>Changed C5, C7, C6</t>
   </si>
 </sst>
 </file>
@@ -415,7 +418,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -593,6 +596,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -757,7 +766,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -765,12 +774,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1116,8 +1131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1152,13 +1167,13 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -1166,7 +1181,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -1177,11 +1192,11 @@
       <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="3">
         <v>0.01</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>65</v>
+      <c r="I2" s="4" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -1200,34 +1215,34 @@
       <c r="E3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>0.01</v>
       </c>
-      <c r="I3" s="5" t="s">
-        <v>56</v>
+      <c r="I3" s="4" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>4</v>
+      <c r="A4" s="6">
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
       </c>
       <c r="C4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>0.1</v>
       </c>
-      <c r="I4" s="5" t="s">
-        <v>60</v>
+      <c r="I4" s="4" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -1235,22 +1250,22 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <v>0.01</v>
       </c>
-      <c r="I5" s="5" t="s">
-        <v>57</v>
+      <c r="I5" s="4" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -1258,45 +1273,45 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>0.01</v>
       </c>
-      <c r="I6" s="5" t="s">
-        <v>47</v>
+      <c r="I6" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>2</v>
+      <c r="A7" s="6">
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E7" t="s">
         <v>14</v>
       </c>
-      <c r="D7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="4">
+      <c r="F7" s="3">
         <v>0.1</v>
       </c>
-      <c r="I7" s="5" t="s">
-        <v>61</v>
+      <c r="I7" s="4" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -1304,22 +1319,22 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E8" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="3">
         <v>0.01</v>
       </c>
-      <c r="I8" s="5" t="s">
-        <v>56</v>
+      <c r="I8" s="4" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -1327,22 +1342,22 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" t="s">
         <v>14</v>
       </c>
-      <c r="D9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="6">
+      <c r="F9" s="5">
         <v>0.1</v>
       </c>
-      <c r="I9" s="5" t="s">
-        <v>59</v>
+      <c r="I9" s="4" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -1350,22 +1365,22 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E10" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="3">
         <v>0.01</v>
       </c>
-      <c r="I10" s="5" t="s">
-        <v>56</v>
+      <c r="I10" s="4" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -1373,22 +1388,22 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E11" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="3">
         <v>0.01</v>
       </c>
-      <c r="I11" s="5" t="s">
-        <v>56</v>
+      <c r="I11" s="4" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -1396,26 +1411,26 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E12" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F12"/>
       <c r="G12" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -1423,20 +1438,20 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D13" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E13" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F13"/>
-      <c r="I13" s="5" t="s">
-        <v>46</v>
+      <c r="I13" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -1444,20 +1459,20 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C14" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D14" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E14" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F14"/>
-      <c r="I14" s="5" t="s">
-        <v>66</v>
+      <c r="I14" s="4" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -1465,20 +1480,20 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E15" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F15"/>
-      <c r="I15" s="5" t="s">
-        <v>48</v>
+      <c r="I15" s="4" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -1486,20 +1501,20 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D16" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E16" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F16"/>
-      <c r="I16" s="5" t="s">
-        <v>75</v>
+      <c r="I16" s="4" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
@@ -1507,16 +1522,16 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C17"/>
       <c r="D17"/>
       <c r="E17" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F17"/>
-      <c r="I17" s="5" t="s">
-        <v>55</v>
+      <c r="I17" s="4" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
@@ -1524,18 +1539,18 @@
         <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C18" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D18"/>
       <c r="E18" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F18"/>
-      <c r="I18" s="5" t="s">
-        <v>62</v>
+      <c r="I18" s="4" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -1543,16 +1558,16 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C19"/>
       <c r="D19"/>
       <c r="E19" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F19"/>
-      <c r="I19" s="5" t="s">
-        <v>72</v>
+      <c r="I19" s="4" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
@@ -1560,16 +1575,16 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C20"/>
       <c r="D20"/>
       <c r="E20" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F20"/>
-      <c r="I20" s="5" t="s">
-        <v>53</v>
+      <c r="I20" s="4" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1601,33 +1616,42 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C3"/>
+  <dimension ref="B2:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.109375" customWidth="1"/>
-    <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="46" customWidth="1"/>
+    <col min="1" max="1" width="3.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10" style="1" customWidth="1"/>
+    <col min="3" max="3" width="46" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C2" t="s">
-        <v>81</v>
-      </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B3" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C3" t="s">
-        <v>80</v>
+      <c r="B3" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4" s="8">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
R2.02 changed opamp to MCP6004-I/SL
</commit_message>
<xml_diff>
--- a/BOM/electronicloadBOM.xlsx
+++ b/BOM/electronicloadBOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="36" windowWidth="22980" windowHeight="9552" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="36" windowWidth="22980" windowHeight="9552"/>
   </bookViews>
   <sheets>
     <sheet name="electronicloadBOM" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="87">
   <si>
     <t>Qty</t>
   </si>
@@ -155,18 +155,6 @@
     <t>http://www.ebay.com/itm/10PCS-HEXFET-Power-MOSFET-IR-TO-220-IRLB3034-IRLB3034PBF-100-Genuine-and-New/361945536225</t>
   </si>
   <si>
-    <t>http://www.ebay.com/itm/10PCS-LMV324IDR-Quad-Op-Amp-Rail-to-Rail-Output-SMD/171907470630</t>
-  </si>
-  <si>
-    <t>LMV324IDR Quad Op-Amp Rail to Rail Output SMD</t>
-  </si>
-  <si>
-    <t>LMV324IDR</t>
-  </si>
-  <si>
-    <t>TI</t>
-  </si>
-  <si>
     <t>http://www.ebay.com/itm/3-Sheets-CE-Certificated-Label-Stickers-Adhesive-Sticker-Markers-Home-Appliance/172533333629</t>
   </si>
   <si>
@@ -267,6 +255,27 @@
   </si>
   <si>
     <t>Changed C5, C7, C6</t>
+  </si>
+  <si>
+    <t>PCB R2</t>
+  </si>
+  <si>
+    <t>Replaced opamp LMV324 with MCP6004-I/SL</t>
+  </si>
+  <si>
+    <t>MCP6004-I/SL</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com/itm/10pcs-MCP6004-I-SL-MCP6004-SOP-14-IC/391914610679</t>
+  </si>
+  <si>
+    <t>Microchip</t>
+  </si>
+  <si>
+    <t>1 MHz, Low-Power Op Amp</t>
+  </si>
+  <si>
+    <t>PCB Jasper's Electronic Load R2</t>
   </si>
 </sst>
 </file>
@@ -766,7 +775,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -784,6 +793,16 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1129,15 +1148,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.88671875" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.33203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="18.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="20" style="1" customWidth="1"/>
@@ -1148,7 +1167,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -1177,11 +1196,11 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="9">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -1196,11 +1215,11 @@
         <v>0.01</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="9">
         <v>1</v>
       </c>
       <c r="B3" t="s">
@@ -1219,21 +1238,21 @@
         <v>0.01</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="6">
+      <c r="A4" s="10">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E4" t="s">
         <v>14</v>
@@ -1242,11 +1261,11 @@
         <v>0.1</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" s="9">
         <v>3</v>
       </c>
       <c r="B5" t="s">
@@ -1265,11 +1284,11 @@
         <v>0.01</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="A6" s="9">
         <v>1</v>
       </c>
       <c r="B6" t="s">
@@ -1292,17 +1311,17 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="6">
+      <c r="A7" s="10">
         <v>4</v>
       </c>
       <c r="B7" t="s">
         <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E7" t="s">
         <v>14</v>
@@ -1311,11 +1330,11 @@
         <v>0.1</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="A8" s="9">
         <v>4</v>
       </c>
       <c r="B8" t="s">
@@ -1325,7 +1344,7 @@
         <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E8" t="s">
         <v>12</v>
@@ -1334,18 +1353,18 @@
         <v>0.01</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="A9" s="9">
         <v>1</v>
       </c>
       <c r="B9" t="s">
         <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D9" t="s">
         <v>20</v>
@@ -1357,11 +1376,11 @@
         <v>0.1</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="A10" s="9">
         <v>1</v>
       </c>
       <c r="B10" t="s">
@@ -1380,11 +1399,11 @@
         <v>0.01</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="A11" s="9">
         <v>3</v>
       </c>
       <c r="B11" t="s">
@@ -1394,7 +1413,7 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E11" t="s">
         <v>12</v>
@@ -1403,15 +1422,15 @@
         <v>0.01</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="A12" s="9">
         <v>1</v>
       </c>
-      <c r="B12" t="s">
-        <v>48</v>
+      <c r="B12" s="11" t="s">
+        <v>82</v>
       </c>
       <c r="C12" t="s">
         <v>24</v>
@@ -1420,21 +1439,21 @@
         <v>25</v>
       </c>
       <c r="E12" t="s">
-        <v>47</v>
+        <v>85</v>
       </c>
       <c r="F12"/>
       <c r="G12" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>48</v>
+        <v>84</v>
+      </c>
+      <c r="H12" t="s">
+        <v>82</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>46</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13">
+      <c r="A13" s="9">
         <v>1</v>
       </c>
       <c r="B13" t="s">
@@ -1447,7 +1466,7 @@
         <v>27</v>
       </c>
       <c r="E13" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F13"/>
       <c r="I13" s="4" t="s">
@@ -1455,28 +1474,28 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14">
+      <c r="A14" s="9">
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C14" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D14" t="s">
         <v>28</v>
       </c>
       <c r="E14" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F14"/>
       <c r="I14" s="4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15">
+      <c r="A15" s="9">
         <v>1</v>
       </c>
       <c r="B15" t="s">
@@ -1489,7 +1508,7 @@
         <v>31</v>
       </c>
       <c r="E15" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F15"/>
       <c r="I15" s="4" t="s">
@@ -1497,11 +1516,11 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16">
+      <c r="A16" s="9">
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C16" t="s">
         <v>32</v>
@@ -1510,15 +1529,15 @@
         <v>33</v>
       </c>
       <c r="E16" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F16"/>
       <c r="I16" s="4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17">
+      <c r="A17" s="9">
         <v>2</v>
       </c>
       <c r="B17" t="s">
@@ -1531,30 +1550,30 @@
       </c>
       <c r="F17"/>
       <c r="I17" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18">
+      <c r="A18" s="9">
         <v>4</v>
       </c>
       <c r="B18" t="s">
         <v>34</v>
       </c>
       <c r="C18" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D18"/>
       <c r="E18" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F18"/>
       <c r="I18" s="4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19">
+      <c r="A19" s="9">
         <v>1</v>
       </c>
       <c r="B19" t="s">
@@ -1563,28 +1582,39 @@
       <c r="C19"/>
       <c r="D19"/>
       <c r="E19" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F19"/>
       <c r="I19" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20">
+      <c r="A20" s="9">
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C20"/>
       <c r="D20"/>
       <c r="E20" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F20"/>
       <c r="I20" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="9">
+        <v>1</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1592,34 +1622,33 @@
     <hyperlink ref="I13" r:id="rId1"/>
     <hyperlink ref="I6" r:id="rId2"/>
     <hyperlink ref="I15" r:id="rId3"/>
-    <hyperlink ref="I12" r:id="rId4"/>
-    <hyperlink ref="I20" r:id="rId5"/>
-    <hyperlink ref="I17" r:id="rId6"/>
-    <hyperlink ref="I10" r:id="rId7"/>
-    <hyperlink ref="I11" r:id="rId8"/>
-    <hyperlink ref="I8" r:id="rId9"/>
-    <hyperlink ref="I3" r:id="rId10"/>
-    <hyperlink ref="I5" r:id="rId11"/>
-    <hyperlink ref="I9" r:id="rId12"/>
-    <hyperlink ref="I4" r:id="rId13"/>
-    <hyperlink ref="I7" r:id="rId14"/>
-    <hyperlink ref="I18" r:id="rId15"/>
-    <hyperlink ref="I2" r:id="rId16"/>
-    <hyperlink ref="I14" r:id="rId17"/>
-    <hyperlink ref="I19" r:id="rId18"/>
-    <hyperlink ref="I16" r:id="rId19"/>
+    <hyperlink ref="I20" r:id="rId4"/>
+    <hyperlink ref="I17" r:id="rId5"/>
+    <hyperlink ref="I10" r:id="rId6"/>
+    <hyperlink ref="I11" r:id="rId7"/>
+    <hyperlink ref="I8" r:id="rId8"/>
+    <hyperlink ref="I3" r:id="rId9"/>
+    <hyperlink ref="I5" r:id="rId10"/>
+    <hyperlink ref="I9" r:id="rId11"/>
+    <hyperlink ref="I4" r:id="rId12"/>
+    <hyperlink ref="I7" r:id="rId13"/>
+    <hyperlink ref="I18" r:id="rId14"/>
+    <hyperlink ref="I2" r:id="rId15"/>
+    <hyperlink ref="I14" r:id="rId16"/>
+    <hyperlink ref="I19" r:id="rId17"/>
+    <hyperlink ref="I16" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId20"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId19"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C4"/>
+  <dimension ref="B2:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1632,18 +1661,18 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.3">
@@ -1651,7 +1680,15 @@
         <v>2.0099999999999998</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>83</v>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B5" s="12">
+        <v>2.02</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2.03 Changed mosfet to the much more robust BTS133
</commit_message>
<xml_diff>
--- a/BOM/electronicloadBOM.xlsx
+++ b/BOM/electronicloadBOM.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="89">
   <si>
     <t>Qty</t>
   </si>
@@ -104,9 +104,6 @@
     <t>X1</t>
   </si>
   <si>
-    <t>IRLB3034PbF</t>
-  </si>
-  <si>
     <t>TO220BV</t>
   </si>
   <si>
@@ -152,9 +149,6 @@
     <t>http://www.ebay.com/itm/100pcs-0603-SMD-Resistor-1-8K-ohm-1K8-Tol-5-RoHS-1-10W/291817476969</t>
   </si>
   <si>
-    <t>http://www.ebay.com/itm/10PCS-HEXFET-Power-MOSFET-IR-TO-220-IRLB3034-IRLB3034PBF-100-Genuine-and-New/361945536225</t>
-  </si>
-  <si>
     <t>http://www.ebay.com/itm/3-Sheets-CE-Certificated-Label-Stickers-Adhesive-Sticker-Markers-Home-Appliance/172533333629</t>
   </si>
   <si>
@@ -242,9 +236,6 @@
     <t>Changes</t>
   </si>
   <si>
-    <t>N-Channel HEXFET Power MOSFET Logic Level</t>
-  </si>
-  <si>
     <t>C1, C3, C5, C6</t>
   </si>
   <si>
@@ -276,6 +267,21 @@
   </si>
   <si>
     <t>PCB Jasper's Electronic Load R2</t>
+  </si>
+  <si>
+    <t>BTS133BKSA1</t>
+  </si>
+  <si>
+    <t>Infineon</t>
+  </si>
+  <si>
+    <t>Smart low side power switch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There's are fake ones on ebay. Please buy from Digikey, Mouser, Farnell etc. </t>
+  </si>
+  <si>
+    <t>Replaced mosfet with BTS133BKSA1</t>
   </si>
 </sst>
 </file>
@@ -775,7 +781,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -805,6 +811,13 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="11" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="11" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="11"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1151,7 +1164,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1186,13 +1199,13 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -1200,7 +1213,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -1215,7 +1228,7 @@
         <v>0.01</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -1238,7 +1251,7 @@
         <v>0.01</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -1249,10 +1262,10 @@
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E4" t="s">
         <v>14</v>
@@ -1261,7 +1274,7 @@
         <v>0.1</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -1269,7 +1282,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
@@ -1284,7 +1297,7 @@
         <v>0.01</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -1292,7 +1305,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
@@ -1307,7 +1320,7 @@
         <v>0.01</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -1318,10 +1331,10 @@
         <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E7" t="s">
         <v>14</v>
@@ -1330,7 +1343,7 @@
         <v>0.1</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -1344,7 +1357,7 @@
         <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E8" t="s">
         <v>12</v>
@@ -1353,7 +1366,7 @@
         <v>0.01</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -1364,7 +1377,7 @@
         <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D9" t="s">
         <v>20</v>
@@ -1376,7 +1389,7 @@
         <v>0.1</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -1399,7 +1412,7 @@
         <v>0.01</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -1413,7 +1426,7 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E11" t="s">
         <v>12</v>
@@ -1422,7 +1435,7 @@
         <v>0.01</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -1430,7 +1443,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C12" t="s">
         <v>24</v>
@@ -1439,17 +1452,17 @@
         <v>25</v>
       </c>
       <c r="E12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F12"/>
       <c r="G12" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H12" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -1466,11 +1479,11 @@
         <v>27</v>
       </c>
       <c r="E13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F13"/>
       <c r="I13" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -1478,41 +1491,47 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D14" t="s">
         <v>28</v>
       </c>
       <c r="E14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F14"/>
       <c r="I14" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="9">
         <v>1</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="C15" t="s">
         <v>29</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>30</v>
       </c>
-      <c r="D15" t="s">
-        <v>31</v>
-      </c>
-      <c r="E15" t="s">
-        <v>75</v>
-      </c>
-      <c r="F15"/>
-      <c r="I15" s="4" t="s">
-        <v>45</v>
+      <c r="E15" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="F15" s="15"/>
+      <c r="G15" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="I15" s="15" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -1520,20 +1539,20 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" t="s">
         <v>32</v>
       </c>
-      <c r="D16" t="s">
-        <v>33</v>
-      </c>
       <c r="E16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F16"/>
       <c r="I16" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
@@ -1541,16 +1560,16 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C17"/>
       <c r="D17"/>
       <c r="E17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F17"/>
       <c r="I17" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
@@ -1558,18 +1577,18 @@
         <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D18"/>
       <c r="E18" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F18"/>
       <c r="I18" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -1577,16 +1596,16 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C19"/>
       <c r="D19"/>
       <c r="E19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F19"/>
       <c r="I19" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
@@ -1594,16 +1613,16 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C20"/>
       <c r="D20"/>
       <c r="E20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F20"/>
       <c r="I20" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
@@ -1611,44 +1630,43 @@
         <v>1</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I13" r:id="rId1"/>
     <hyperlink ref="I6" r:id="rId2"/>
-    <hyperlink ref="I15" r:id="rId3"/>
-    <hyperlink ref="I20" r:id="rId4"/>
-    <hyperlink ref="I17" r:id="rId5"/>
-    <hyperlink ref="I10" r:id="rId6"/>
-    <hyperlink ref="I11" r:id="rId7"/>
-    <hyperlink ref="I8" r:id="rId8"/>
-    <hyperlink ref="I3" r:id="rId9"/>
-    <hyperlink ref="I5" r:id="rId10"/>
-    <hyperlink ref="I9" r:id="rId11"/>
-    <hyperlink ref="I4" r:id="rId12"/>
-    <hyperlink ref="I7" r:id="rId13"/>
-    <hyperlink ref="I18" r:id="rId14"/>
-    <hyperlink ref="I2" r:id="rId15"/>
-    <hyperlink ref="I14" r:id="rId16"/>
-    <hyperlink ref="I19" r:id="rId17"/>
-    <hyperlink ref="I16" r:id="rId18"/>
+    <hyperlink ref="I20" r:id="rId3"/>
+    <hyperlink ref="I17" r:id="rId4"/>
+    <hyperlink ref="I10" r:id="rId5"/>
+    <hyperlink ref="I11" r:id="rId6"/>
+    <hyperlink ref="I8" r:id="rId7"/>
+    <hyperlink ref="I3" r:id="rId8"/>
+    <hyperlink ref="I5" r:id="rId9"/>
+    <hyperlink ref="I9" r:id="rId10"/>
+    <hyperlink ref="I4" r:id="rId11"/>
+    <hyperlink ref="I7" r:id="rId12"/>
+    <hyperlink ref="I18" r:id="rId13"/>
+    <hyperlink ref="I2" r:id="rId14"/>
+    <hyperlink ref="I14" r:id="rId15"/>
+    <hyperlink ref="I19" r:id="rId16"/>
+    <hyperlink ref="I16" r:id="rId17"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId19"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId18"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C5"/>
+  <dimension ref="B2:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:C5"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1661,18 +1679,18 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.3">
@@ -1680,7 +1698,7 @@
         <v>2.0099999999999998</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.3">
@@ -1688,7 +1706,15 @@
         <v>2.02</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>81</v>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B6" s="13">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed opamp from MCP6004 to MCP6074 (much lower input voltage offset)
</commit_message>
<xml_diff>
--- a/BOM/electronicloadBOM.xlsx
+++ b/BOM/electronicloadBOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="36" windowWidth="22980" windowHeight="9552"/>
+    <workbookView xWindow="0" yWindow="36" windowWidth="22980" windowHeight="9552" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="electronicloadBOM" sheetId="1" r:id="rId1"/>
@@ -254,18 +254,9 @@
     <t>Replaced opamp LMV324 with MCP6004-I/SL</t>
   </si>
   <si>
-    <t>MCP6004-I/SL</t>
-  </si>
-  <si>
-    <t>https://www.ebay.com/itm/10pcs-MCP6004-I-SL-MCP6004-SOP-14-IC/391914610679</t>
-  </si>
-  <si>
     <t>Microchip</t>
   </si>
   <si>
-    <t>1 MHz, Low-Power Op Amp</t>
-  </si>
-  <si>
     <t>PCB Jasper's Electronic Load R2</t>
   </si>
   <si>
@@ -282,6 +273,15 @@
   </si>
   <si>
     <t>Replaced mosfet with BTS133BKSA1</t>
+  </si>
+  <si>
+    <t>MCP6074-E/SL</t>
+  </si>
+  <si>
+    <t>Op Amp</t>
+  </si>
+  <si>
+    <t>Changed opamp MCP4006 with MCP6074-E/SL</t>
   </si>
 </sst>
 </file>
@@ -1163,8 +1163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1443,7 +1443,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="C12" t="s">
         <v>24</v>
@@ -1452,18 +1452,16 @@
         <v>25</v>
       </c>
       <c r="E12" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="F12"/>
       <c r="G12" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="H12" t="s">
         <v>79</v>
       </c>
-      <c r="I12" s="4" t="s">
-        <v>80</v>
-      </c>
+      <c r="H12" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="I12" s="4"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="9">
@@ -1512,7 +1510,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C15" t="s">
         <v>29</v>
@@ -1521,17 +1519,17 @@
         <v>30</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F15" s="15"/>
       <c r="G15" s="13" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H15" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="I15" s="15" t="s">
         <v>84</v>
-      </c>
-      <c r="I15" s="15" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -1633,7 +1631,7 @@
         <v>77</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1663,10 +1661,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C6"/>
+  <dimension ref="B2:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1714,6 +1712,14 @@
         <v>2.0299999999999998</v>
       </c>
       <c r="C6" s="13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B7" s="1">
+        <v>2.04</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>88</v>
       </c>
     </row>

</xml_diff>

<commit_message>
R2.1 New PCB design, added USB connector, changed mosfet from MCP6004 to MCP6074-E/SL
</commit_message>
<xml_diff>
--- a/BOM/electronicloadBOM.xlsx
+++ b/BOM/electronicloadBOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="36" windowWidth="22980" windowHeight="9552" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="36" windowWidth="22980" windowHeight="9552"/>
   </bookViews>
   <sheets>
     <sheet name="electronicloadBOM" sheetId="1" r:id="rId1"/>
@@ -1163,7 +1163,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -1663,7 +1663,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -1717,7 +1717,7 @@
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B7" s="1">
-        <v>2.04</v>
+        <v>2.1</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>88</v>

</xml_diff>

<commit_message>
BOM R2.1.1 Added extra large heat sink (31W) to the BOM
</commit_message>
<xml_diff>
--- a/BOM/electronicloadBOM.xlsx
+++ b/BOM/electronicloadBOM.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Jasper\electronica\electronic load\R2\eagle\R2.1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="36" windowWidth="22980" windowHeight="9552"/>
+    <workbookView xWindow="0" yWindow="36" windowWidth="22980" windowHeight="9552" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="electronicloadBOM" sheetId="1" r:id="rId1"/>
@@ -15,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="95">
   <si>
     <t>Qty</t>
   </si>
@@ -281,13 +286,31 @@
     <t>Op Amp</t>
   </si>
   <si>
-    <t>Changed opamp MCP4006 with MCP6074-E/SL</t>
+    <t>Replaced opamp MCP4006 with MCP6074-E/SL</t>
+  </si>
+  <si>
+    <t>Added option for 31W heat sink</t>
+  </si>
+  <si>
+    <t>AAVID THERMALLOY</t>
+  </si>
+  <si>
+    <t>530002B02500G</t>
+  </si>
+  <si>
+    <t>http://nl.farnell.com/aavid-thermalloy/530002b02500g/heat-sink-2-6k-w-to-220/dp/2295719</t>
+  </si>
+  <si>
+    <t>Aluminum Heatsink H=63.5mm 42x25x63mm Black TO-TO-220</t>
+  </si>
+  <si>
+    <t>KK1-alternative</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -781,7 +804,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -795,12 +818,6 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -808,9 +825,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="11" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -818,6 +832,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="11"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="11" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -870,6 +894,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -917,7 +944,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -950,9 +977,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -985,6 +1029,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1161,15 +1222,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.88671875" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.33203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="18.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="20" style="1" customWidth="1"/>
@@ -1180,7 +1241,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -1209,7 +1270,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="9">
+      <c r="A2" s="7">
         <v>3</v>
       </c>
       <c r="B2" t="s">
@@ -1232,7 +1293,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="9">
+      <c r="A3" s="7">
         <v>1</v>
       </c>
       <c r="B3" t="s">
@@ -1255,7 +1316,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="10">
+      <c r="A4" s="8">
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -1278,7 +1339,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="9">
+      <c r="A5" s="7">
         <v>3</v>
       </c>
       <c r="B5" t="s">
@@ -1301,7 +1362,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="9">
+      <c r="A6" s="7">
         <v>1</v>
       </c>
       <c r="B6" t="s">
@@ -1324,7 +1385,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="10">
+      <c r="A7" s="8">
         <v>4</v>
       </c>
       <c r="B7" t="s">
@@ -1347,7 +1408,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="9">
+      <c r="A8" s="7">
         <v>4</v>
       </c>
       <c r="B8" t="s">
@@ -1370,7 +1431,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="9">
+      <c r="A9" s="7">
         <v>1</v>
       </c>
       <c r="B9" t="s">
@@ -1393,7 +1454,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="9">
+      <c r="A10" s="7">
         <v>1</v>
       </c>
       <c r="B10" t="s">
@@ -1416,7 +1477,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="9">
+      <c r="A11" s="7">
         <v>3</v>
       </c>
       <c r="B11" t="s">
@@ -1439,10 +1500,10 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="9">
+      <c r="A12" s="7">
         <v>1</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="9" t="s">
         <v>86</v>
       </c>
       <c r="C12" t="s">
@@ -1458,13 +1519,13 @@
       <c r="G12" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H12" s="11" t="s">
+      <c r="H12" s="9" t="s">
         <v>86</v>
       </c>
       <c r="I12" s="4"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="9">
+      <c r="A13" s="7">
         <v>1</v>
       </c>
       <c r="B13" t="s">
@@ -1485,7 +1546,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="9">
+      <c r="A14" s="7">
         <v>1</v>
       </c>
       <c r="B14" t="s">
@@ -1506,10 +1567,10 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="9">
+      <c r="A15" s="7">
         <v>1</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="11" t="s">
         <v>81</v>
       </c>
       <c r="C15" t="s">
@@ -1518,22 +1579,22 @@
       <c r="D15" t="s">
         <v>30</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="E15" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="F15" s="15"/>
-      <c r="G15" s="13" t="s">
+      <c r="F15" s="12"/>
+      <c r="G15" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="H15" s="13" t="s">
+      <c r="H15" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="I15" s="15" t="s">
+      <c r="I15" s="12" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="9">
+      <c r="A16" s="7">
         <v>1</v>
       </c>
       <c r="B16" t="s">
@@ -1554,83 +1615,110 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="9">
+      <c r="A17" s="7">
+        <v>1</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="F17" s="19"/>
+      <c r="G17" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="H17" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="7">
         <v>2</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>37</v>
       </c>
-      <c r="C17"/>
-      <c r="D17"/>
-      <c r="E17" t="s">
-        <v>36</v>
-      </c>
-      <c r="F17"/>
-      <c r="I17" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="9">
-        <v>4</v>
-      </c>
-      <c r="B18" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" t="s">
-        <v>55</v>
-      </c>
+      <c r="C18"/>
       <c r="D18"/>
       <c r="E18" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="F18"/>
       <c r="I18" s="4" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="9">
-        <v>1</v>
+      <c r="A19" s="7">
+        <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19"/>
+        <v>33</v>
+      </c>
+      <c r="C19" t="s">
+        <v>55</v>
+      </c>
       <c r="D19"/>
       <c r="E19" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="F19"/>
       <c r="I19" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="9">
+      <c r="A20" s="7">
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="C20"/>
       <c r="D20"/>
       <c r="E20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F20"/>
       <c r="I20" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="7">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21"/>
+      <c r="D21"/>
+      <c r="E21" t="s">
+        <v>65</v>
+      </c>
+      <c r="F21"/>
+      <c r="I21" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="7">
         <v>1</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1638,8 +1726,8 @@
   <hyperlinks>
     <hyperlink ref="I13" r:id="rId1"/>
     <hyperlink ref="I6" r:id="rId2"/>
-    <hyperlink ref="I20" r:id="rId3"/>
-    <hyperlink ref="I17" r:id="rId4"/>
+    <hyperlink ref="I21" r:id="rId3"/>
+    <hyperlink ref="I18" r:id="rId4"/>
     <hyperlink ref="I10" r:id="rId5"/>
     <hyperlink ref="I11" r:id="rId6"/>
     <hyperlink ref="I8" r:id="rId7"/>
@@ -1648,79 +1736,88 @@
     <hyperlink ref="I9" r:id="rId10"/>
     <hyperlink ref="I4" r:id="rId11"/>
     <hyperlink ref="I7" r:id="rId12"/>
-    <hyperlink ref="I18" r:id="rId13"/>
+    <hyperlink ref="I19" r:id="rId13"/>
     <hyperlink ref="I2" r:id="rId14"/>
     <hyperlink ref="I14" r:id="rId15"/>
-    <hyperlink ref="I19" r:id="rId16"/>
+    <hyperlink ref="I20" r:id="rId16"/>
     <hyperlink ref="I16" r:id="rId17"/>
+    <hyperlink ref="I17" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId18"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId19"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C7"/>
+  <dimension ref="B2:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10" style="1" customWidth="1"/>
-    <col min="3" max="3" width="46" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="3.109375" style="13" customWidth="1"/>
+    <col min="2" max="2" width="10" style="13" customWidth="1"/>
+    <col min="3" max="3" width="46" style="13" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="13"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="13" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="13" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B4" s="8">
+      <c r="B4" s="15">
         <v>2.0099999999999998</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="15" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B5" s="12">
+      <c r="B5" s="13">
         <v>2.02</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="13" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B6" s="13">
+      <c r="B6" s="16">
         <v>2.0299999999999998</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="16" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B7" s="1">
+      <c r="B7" s="17">
         <v>2.1</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="17" t="s">
         <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B8" s="18">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>